<commit_message>
finished adding data for yahoo
</commit_message>
<xml_diff>
--- a/data_formatted/yahoo2007.xlsx
+++ b/data_formatted/yahoo2007.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="19000" yWindow="60" windowWidth="13760" windowHeight="22600" tabRatio="500"/>
+    <workbookView xWindow="19900" yWindow="-80" windowWidth="13760" windowHeight="22600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,183 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+  <si>
+    <t>Muhammad | Muhsin</t>
+  </si>
+  <si>
+    <t>Bruce | Isaac</t>
+  </si>
+  <si>
+    <t>Curry | Ronald</t>
+  </si>
+  <si>
+    <t>Bennett | Drew</t>
+  </si>
+  <si>
+    <t>Marshall | Brandon</t>
+  </si>
+  <si>
+    <t>Horn | Joe</t>
+  </si>
+  <si>
+    <t>Kennison | Eddie</t>
+  </si>
+  <si>
+    <t>Gonzalez | Anthony</t>
+  </si>
+  <si>
+    <t>Furrey | Mike</t>
+  </si>
+  <si>
+    <t>Mason | Derrick</t>
+  </si>
+  <si>
+    <t>Jones | Jacoby</t>
+  </si>
+  <si>
+    <t>Williams | Demetrius</t>
+  </si>
+  <si>
+    <t>Welker | Wes</t>
+  </si>
+  <si>
+    <t>Jones | James</t>
+  </si>
+  <si>
+    <t>Bowe | Dwayne</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jones | Matt</t>
+  </si>
+  <si>
+    <t>Wilford | Ernest</t>
+  </si>
+  <si>
+    <t>Wade | Bobby</t>
+  </si>
+  <si>
+    <t>Smith | Steve (Car)</t>
+  </si>
+  <si>
+    <t>Harrison | Marvin</t>
+  </si>
+  <si>
+    <t>Johnson | Chad</t>
+  </si>
+  <si>
+    <t>Owens | Terrell</t>
+  </si>
+  <si>
+    <t>Wayne | Reggie</t>
+  </si>
+  <si>
+    <t>Holt | Torry</t>
+  </si>
+  <si>
+    <t>Fitzgerald | Larry</t>
+  </si>
+  <si>
+    <t>Houshmandzadeh | T.J.</t>
+  </si>
+  <si>
+    <t>Colston | Marques</t>
+  </si>
+  <si>
+    <t>Walker | Javon</t>
+  </si>
+  <si>
+    <t>Evans | Lee</t>
+  </si>
+  <si>
+    <t>Boldin | Anquan</t>
+  </si>
+  <si>
+    <t>Williams | Roy</t>
+  </si>
+  <si>
+    <t>Johnson | Andre</t>
+  </si>
+  <si>
+    <t>Moss | Randy</t>
+  </si>
+  <si>
+    <t>Driver | Donald</t>
+  </si>
+  <si>
+    <t>Burress | Plaxico</t>
+  </si>
+  <si>
+    <t>Ward | Hines</t>
+  </si>
+  <si>
+    <t>Brown | Reggie</t>
+  </si>
+  <si>
+    <t>Coles | Laveranues</t>
+  </si>
+  <si>
+    <t>Johnson | Calvin</t>
+  </si>
+  <si>
+    <t>Moss | Santana</t>
+  </si>
+  <si>
+    <t>Branch | Deion</t>
+  </si>
+  <si>
+    <t>Edwards | Braylon</t>
+  </si>
+  <si>
+    <t>Galloway | Joey</t>
+  </si>
+  <si>
+    <t>Jackson | Darrell</t>
+  </si>
+  <si>
+    <t>Cotchery | Jerricho</t>
+  </si>
+  <si>
+    <t>Jackson | Vincent</t>
+  </si>
+  <si>
+    <t>Clayton | Mark</t>
+  </si>
+  <si>
+    <t>Berrian | Bernard</t>
+  </si>
+  <si>
+    <t>Chambers | Chris</t>
+  </si>
+  <si>
+    <t>Holmes | Santonio</t>
+  </si>
+  <si>
+    <t>Henderson | Devery</t>
+  </si>
+  <si>
+    <t>Glenn | Terry</t>
+  </si>
+  <si>
+    <t>Stallworth | Donte</t>
+  </si>
+  <si>
+    <t>Curtis | Kevin</t>
+  </si>
+  <si>
+    <t>Hackett | D.J.</t>
+  </si>
+  <si>
+    <t>Jennings | Greg</t>
+  </si>
+  <si>
+    <t>Porter | Jerry</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -390,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="C1:C50"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -402,155 +579,511 @@
     <col min="3" max="3" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:3">
+    <row r="1" spans="1:3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="3:3">
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="3:3">
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="3:3">
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="3:3">
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="3:3">
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="3:3">
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="3:3">
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="3:3">
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="3:3">
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="3:3">
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="3:3">
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="3:3">
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="3:3">
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="3:3">
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="3:3">
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="3:3">
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="3:3">
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="3:3">
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="3:3">
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="3:3">
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="3:3">
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="3:3">
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="3:3">
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="3:3">
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="3:3">
+    <row r="26" spans="1:3">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="3:3">
+    <row r="27" spans="1:3">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="3:3">
+    <row r="28" spans="1:3">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="3:3">
+    <row r="29" spans="1:3">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="3:3">
+    <row r="30" spans="1:3">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="3:3">
+    <row r="31" spans="1:3">
+      <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="3:3">
+    <row r="32" spans="1:3">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="3:3">
+    <row r="33" spans="1:3">
+      <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="3:3">
+    <row r="34" spans="1:3">
+      <c r="A34">
+        <v>34</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="3:3">
+    <row r="35" spans="1:3">
+      <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="3:3">
+    <row r="36" spans="1:3">
+      <c r="A36">
+        <v>36</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="3:3">
+    <row r="37" spans="1:3">
+      <c r="A37">
+        <v>37</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="3:3">
+    <row r="38" spans="1:3">
+      <c r="A38">
+        <v>38</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="3:3">
+    <row r="39" spans="1:3">
+      <c r="A39">
+        <v>39</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="3:3">
+    <row r="40" spans="1:3">
+      <c r="A40">
+        <v>40</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="3:3">
+    <row r="41" spans="1:3">
+      <c r="A41">
+        <v>41</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="3:3">
+    <row r="42" spans="1:3">
+      <c r="A42">
+        <v>42</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="3:3">
+    <row r="43" spans="1:3">
+      <c r="A43">
+        <v>43</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="3:3">
+    <row r="44" spans="1:3">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="3:3">
+    <row r="45" spans="1:3">
+      <c r="A45">
+        <v>45</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="3:3">
+    <row r="46" spans="1:3">
+      <c r="A46">
+        <v>46</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="3:3">
+    <row r="47" spans="1:3">
+      <c r="A47">
+        <v>47</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="3:3">
+    <row r="48" spans="1:3">
+      <c r="A48">
+        <v>48</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="C48" s="1"/>
     </row>
-    <row r="49" spans="3:3">
+    <row r="49" spans="1:3">
+      <c r="A49">
+        <v>49</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="C49" s="1"/>
     </row>
-    <row r="50" spans="3:3">
+    <row r="50" spans="1:3">
+      <c r="A50">
+        <v>50</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="C50" s="1"/>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51">
+        <v>51</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52">
+        <v>52</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53">
+        <v>53</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54">
+        <v>54</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55">
+        <v>55</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56">
+        <v>56</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57">
+        <v>57</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>